<commit_message>
Update Requirement Gathering process(MOM).xlsx
</commit_message>
<xml_diff>
--- a/Aurora/Requirements/User Stories/Requirement Gathering process(MOM).xlsx
+++ b/Aurora/Requirements/User Stories/Requirement Gathering process(MOM).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25301"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ADE3233-1F5D-42E4-A52D-4A0ECDDF9D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FA07415-0965-4AB2-A539-A5887A3A8114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day1   04.04.2022" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,8 @@
     <sheet name="Day 14 22.04.2022  " sheetId="15" r:id="rId14"/>
     <sheet name="Day 15 23.04.2022  " sheetId="16" r:id="rId15"/>
     <sheet name="Day 17 26.04.2022  " sheetId="17" r:id="rId16"/>
-    <sheet name="Day 26 05.05.2022   " sheetId="18" r:id="rId17"/>
+    <sheet name="06.05.2022" sheetId="19" r:id="rId17"/>
+    <sheet name="Day 26 05.05.2022   " sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="458">
   <si>
     <t>Actors</t>
   </si>
@@ -1754,6 +1755,21 @@
   </si>
   <si>
     <t>in Admin Side, Users to be verified header should be changed</t>
+  </si>
+  <si>
+    <t>Minutes of Meeting</t>
+  </si>
+  <si>
+    <t>1.Sequence Diagram Should be include all the codes.</t>
+  </si>
+  <si>
+    <t>2.Need to work on userservice</t>
+  </si>
+  <si>
+    <t>3.send mail to rafi (logfile)</t>
+  </si>
+  <si>
+    <t>4.Proper Exception</t>
   </si>
   <si>
     <t>Day 26-Minutes of Meeting</t>
@@ -1981,7 +1997,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2066,6 +2082,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6DCE4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2088,7 +2110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2149,6 +2171,8 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9883,7 +9907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52731B6-8B14-4651-BA9B-3F09729F59CE}">
   <dimension ref="A1:AB134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F14" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
@@ -10859,6 +10883,76 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDBDB3A-70A7-45E1-BF98-AC2E116C3A2E}">
+  <dimension ref="E7:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="7" spans="5:11" ht="18.75">
+      <c r="E7" s="55" t="s">
+        <v>441</v>
+      </c>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+    </row>
+    <row r="8" spans="5:11" ht="18.75">
+      <c r="E8" s="55" t="s">
+        <v>442</v>
+      </c>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+    </row>
+    <row r="9" spans="5:11" ht="18.75">
+      <c r="E9" s="55" t="s">
+        <v>443</v>
+      </c>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+    </row>
+    <row r="10" spans="5:11" ht="18.75">
+      <c r="E10" s="55" t="s">
+        <v>444</v>
+      </c>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+    </row>
+    <row r="11" spans="5:11" ht="18.75">
+      <c r="E11" s="55" t="s">
+        <v>445</v>
+      </c>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4829F6B5-0149-40C8-AC8D-36CD937DDD65}">
   <dimension ref="A1:AB134"/>
   <sheetViews>
@@ -10950,7 +11044,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="33"/>
       <c r="N4" s="12" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="O4" s="50"/>
       <c r="P4" s="11"/>
@@ -11012,7 +11106,7 @@
         <v>1</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
@@ -11042,7 +11136,7 @@
         <v>2</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
@@ -11082,7 +11176,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="M8" s="11"/>
       <c r="N8" s="43"/>
@@ -11122,7 +11216,7 @@
         <v>4</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
@@ -11152,7 +11246,7 @@
         <v>5</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
@@ -11182,7 +11276,7 @@
         <v>6</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
@@ -11212,7 +11306,7 @@
         <v>7</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -11242,7 +11336,7 @@
         <v>8</v>
       </c>
       <c r="L13" s="43" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="M13" s="43"/>
       <c r="N13" s="43"/>
@@ -11272,7 +11366,7 @@
         <v>9</v>
       </c>
       <c r="L14" s="43" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="M14" s="43"/>
       <c r="N14" s="43"/>
@@ -11304,7 +11398,7 @@
         <v>10</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
@@ -11344,7 +11438,7 @@
         <v>11</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>

</xml_diff>